<commit_message>
Switching data to another sheet to test
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/testing-job-tracking-parrt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasdecavel/UNIVERSITY OF SAN FRANCISCO/testing_tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B11813A-4768-DA43-89A7-67AE2D8C422B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC47B692-3469-3E42-81EB-C5B946E73E03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="3800" windowWidth="33040" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37300" yWindow="-2780" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -1249,10 +1249,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2172,18 +2186,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>